<commit_message>
added export applied students func
</commit_message>
<xml_diff>
--- a/api/student/test.xlsx
+++ b/api/student/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>name</t>
   </si>
@@ -28,7 +28,7 @@
     <t>division</t>
   </si>
   <si>
-    <t>branch</t>
+    <t>branch_id</t>
   </si>
   <si>
     <t>govind vishwas parulekar</t>
@@ -40,9 +40,6 @@
     <t>jad</t>
   </si>
   <si>
-    <t>adffd</t>
-  </si>
-  <si>
     <t>sunny sit ghat</t>
   </si>
   <si>
@@ -52,9 +49,6 @@
     <t>kjhk</t>
   </si>
   <si>
-    <t>kjh</t>
-  </si>
-  <si>
     <t>some soe foifsdf</t>
   </si>
   <si>
@@ -64,7 +58,40 @@
     <t>hk</t>
   </si>
   <si>
-    <t>khk</t>
+    <t>mike wheeler</t>
+  </si>
+  <si>
+    <t>mike@gmail.com</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>stan pun lee</t>
+  </si>
+  <si>
+    <t>stan@gmail.com</t>
+  </si>
+  <si>
+    <t>sh</t>
+  </si>
+  <si>
+    <t>chin kun jho</t>
+  </si>
+  <si>
+    <t>ching@gmail.com</t>
+  </si>
+  <si>
+    <t>nk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mao li ko </t>
+  </si>
+  <si>
+    <t>mao@gmail.com</t>
+  </si>
+  <si>
+    <t>jd</t>
   </si>
 </sst>
 </file>
@@ -72,10 +99,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -108,29 +135,43 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -138,7 +179,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -146,7 +187,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -160,6 +201,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
@@ -175,45 +224,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -221,22 +264,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -251,6 +278,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -263,55 +326,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,7 +428,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,103 +458,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,16 +473,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -499,11 +535,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -513,21 +555,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -545,148 +572,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -956,13 +983,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="7" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="24.3333333333333" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
@@ -1001,42 +1028,110 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
+      <c r="E2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:5">
       <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="C3" s="1">
         <v>98</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:5">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>78</v>
       </c>
       <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customHeight="1" spans="1:5">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="C5">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" spans="1:5">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>987</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customHeight="1" spans="1:5">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>87</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" customHeight="1" spans="1:5">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>990</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1044,6 +1139,10 @@
     <hyperlink ref="B2" r:id="rId1" display="official5111999@gmail.com" tooltip="mailto:official5111999@gmail.com"/>
     <hyperlink ref="B3" r:id="rId2" display="playgame5111999@gmail.com"/>
     <hyperlink ref="B4" r:id="rId3" display="devgovind511@gmail.com" tooltip="mailto:devgovind511@gmail.com"/>
+    <hyperlink ref="B5" r:id="rId4" display="mike@gmail.com"/>
+    <hyperlink ref="B6" r:id="rId5" display="stan@gmail.com"/>
+    <hyperlink ref="B7" r:id="rId6" display="ching@gmail.com"/>
+    <hyperlink ref="B8" r:id="rId7" display="mao@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>